<commit_message>
Changed how Lat and Long work, and gave each their own column to make the coding easier.
</commit_message>
<xml_diff>
--- a/EATSpointe.xlsx
+++ b/EATSpointe.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\EATSpointe\trunk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cardi\SkyDrive\RokPte\EATSpointe\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988"/>
   </bookViews>
   <sheets>
     <sheet name="EATSpointe" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="231">
   <si>
     <t>Restaurant</t>
   </si>
@@ -233,27 +233,12 @@
     <t>22241 Kelly Road</t>
   </si>
   <si>
-    <t>Lat/Lng</t>
-  </si>
-  <si>
-    <t>42.462028, -82.930547</t>
-  </si>
-  <si>
-    <t>42.464322, -82.959707</t>
-  </si>
-  <si>
     <t>22661 Gratiot Avenue</t>
   </si>
   <si>
-    <t>42.463848, -82.959658</t>
-  </si>
-  <si>
     <t>22611 Gratiot Avenue</t>
   </si>
   <si>
-    <t>42.479991, -82.921896</t>
-  </si>
-  <si>
     <t>19080 East 10 Mile Road</t>
   </si>
   <si>
@@ -263,75 +248,12 @@
     <t>17921 East 9 Mile Road</t>
   </si>
   <si>
-    <t>42.464667, -82.944054</t>
-  </si>
-  <si>
     <t>17210 East 9 Mile Road</t>
   </si>
   <si>
-    <t>42.478462, -82.949634</t>
-  </si>
-  <si>
-    <t>42.465577, -82.935909</t>
-  </si>
-  <si>
-    <t>42.463503, -82.928942</t>
-  </si>
-  <si>
-    <t>42.480217, -82.948572</t>
-  </si>
-  <si>
-    <t>42.472043, -82.952674</t>
-  </si>
-  <si>
-    <t>42.479889, -82.927846</t>
-  </si>
-  <si>
-    <t>42.454643, -82.965264</t>
-  </si>
-  <si>
-    <t>42.474663, -82.952055</t>
-  </si>
-  <si>
-    <t>42.465112, -82.948927</t>
-  </si>
-  <si>
-    <t>42.470411, -82.954819</t>
-  </si>
-  <si>
-    <t>42.465559, -82.958383</t>
-  </si>
-  <si>
-    <t>42.456316, -82.962807</t>
-  </si>
-  <si>
-    <t>42.450935, -82.940886</t>
-  </si>
-  <si>
-    <t>42.450942, -82.966426</t>
-  </si>
-  <si>
-    <t>42.462667, -82.929915</t>
-  </si>
-  <si>
-    <t>42.479804, -82.920525</t>
-  </si>
-  <si>
     <t>Dairy Queen Brazier</t>
   </si>
   <si>
-    <t>42.465111, -82.944537</t>
-  </si>
-  <si>
-    <t>42.479924, -82.964993</t>
-  </si>
-  <si>
-    <t>42.465298, -82.924711</t>
-  </si>
-  <si>
-    <t>42.464157, -82.959707</t>
-  </si>
-  <si>
     <t>East Detroit Bakery</t>
   </si>
   <si>
@@ -344,117 +266,15 @@
     <t>Bakery</t>
   </si>
   <si>
-    <t>42.458315, -82.934028</t>
-  </si>
-  <si>
-    <t>42.462424, -82.958903</t>
-  </si>
-  <si>
-    <t>42.471669, -82.952741</t>
-  </si>
-  <si>
-    <t>42.479976, -82.918491</t>
-  </si>
-  <si>
-    <t>42.479825, -82.958237</t>
-  </si>
-  <si>
     <t>Marz Bar</t>
   </si>
   <si>
-    <t>42.479803, -82.964470</t>
-  </si>
-  <si>
-    <t>42.465404, -82.937518</t>
-  </si>
-  <si>
-    <t>42.479923, -82.955558</t>
-  </si>
-  <si>
-    <t>42.459181, -82.961050</t>
-  </si>
-  <si>
-    <t>42.479876, -82.956645</t>
-  </si>
-  <si>
-    <t>42.453855, -82.938276</t>
-  </si>
-  <si>
-    <t>42.465058, -82.931126</t>
-  </si>
-  <si>
-    <t>42.465148, -82.928295</t>
-  </si>
-  <si>
-    <t>42.480226, -82.955936</t>
-  </si>
-  <si>
-    <t>42.479489, -82.948824</t>
-  </si>
-  <si>
-    <t>42.460782, -82.960984</t>
-  </si>
-  <si>
-    <t>42.459500, -82.932982</t>
-  </si>
-  <si>
-    <t>42.465146, -82.929948</t>
-  </si>
-  <si>
-    <t>42.463094, -82.960277</t>
-  </si>
-  <si>
-    <t>42.465354, -82.938304</t>
-  </si>
-  <si>
-    <t>42.450736, -82.942593</t>
-  </si>
-  <si>
-    <t>42.465537, -82.934832</t>
-  </si>
-  <si>
-    <t>42.456441, -82.963968</t>
-  </si>
-  <si>
-    <t>42.450380, -82.968444</t>
-  </si>
-  <si>
-    <t>42.465453, -82.937006</t>
-  </si>
-  <si>
-    <t>42.463214, -82.960226</t>
-  </si>
-  <si>
-    <t>42.465341, -82.943988</t>
-  </si>
-  <si>
-    <t>42.464982, -82.935152</t>
-  </si>
-  <si>
-    <t>42.465000, -82.932341</t>
-  </si>
-  <si>
-    <t>42.465315, -82.924976</t>
-  </si>
-  <si>
-    <t>42.480257, -82.949271</t>
-  </si>
-  <si>
-    <t>42.464771, -82.941100</t>
-  </si>
-  <si>
     <t>Cup Cakes &amp; Ice Cream Kids</t>
   </si>
   <si>
-    <t>42.464743, -82.940718</t>
-  </si>
-  <si>
     <t>&amp;apos;</t>
   </si>
   <si>
-    <t>42.472294, -82.967218</t>
-  </si>
-  <si>
     <t>Taormina&amp;apos;s Pizza &amp; Ice Cream</t>
   </si>
   <si>
@@ -540,6 +360,363 @@
   </si>
   <si>
     <t>CODE</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lng</t>
+  </si>
+  <si>
+    <t>42.474663</t>
+  </si>
+  <si>
+    <t>42.454643</t>
+  </si>
+  <si>
+    <t>42.479889</t>
+  </si>
+  <si>
+    <t>42.472043</t>
+  </si>
+  <si>
+    <t>42.480217</t>
+  </si>
+  <si>
+    <t>42.463503</t>
+  </si>
+  <si>
+    <t>42.465577</t>
+  </si>
+  <si>
+    <t>42.478462</t>
+  </si>
+  <si>
+    <t>42.462028</t>
+  </si>
+  <si>
+    <t>42.464322</t>
+  </si>
+  <si>
+    <t>42.463848</t>
+  </si>
+  <si>
+    <t>42.479991</t>
+  </si>
+  <si>
+    <t>42.464667</t>
+  </si>
+  <si>
+    <t>42.465112</t>
+  </si>
+  <si>
+    <t>42.470411</t>
+  </si>
+  <si>
+    <t>42.465559</t>
+  </si>
+  <si>
+    <t>42.456316</t>
+  </si>
+  <si>
+    <t>42.450935</t>
+  </si>
+  <si>
+    <t>42.450942</t>
+  </si>
+  <si>
+    <t>42.462667</t>
+  </si>
+  <si>
+    <t>42.479804</t>
+  </si>
+  <si>
+    <t>42.465111</t>
+  </si>
+  <si>
+    <t>42.479924</t>
+  </si>
+  <si>
+    <t>42.465298</t>
+  </si>
+  <si>
+    <t>42.464157</t>
+  </si>
+  <si>
+    <t>42.458315</t>
+  </si>
+  <si>
+    <t>42.462424</t>
+  </si>
+  <si>
+    <t>42.471669</t>
+  </si>
+  <si>
+    <t>-82.952055</t>
+  </si>
+  <si>
+    <t>-82.965264</t>
+  </si>
+  <si>
+    <t>-82.927846</t>
+  </si>
+  <si>
+    <t>-82.952674</t>
+  </si>
+  <si>
+    <t>-82.948572</t>
+  </si>
+  <si>
+    <t>-82.928942</t>
+  </si>
+  <si>
+    <t>-82.935909</t>
+  </si>
+  <si>
+    <t>-82.949634</t>
+  </si>
+  <si>
+    <t>-82.930547</t>
+  </si>
+  <si>
+    <t>-82.959707</t>
+  </si>
+  <si>
+    <t>-82.959658</t>
+  </si>
+  <si>
+    <t>-82.921896</t>
+  </si>
+  <si>
+    <t>-82.944054</t>
+  </si>
+  <si>
+    <t>-82.948927</t>
+  </si>
+  <si>
+    <t>-82.954819</t>
+  </si>
+  <si>
+    <t>-82.958383</t>
+  </si>
+  <si>
+    <t>-82.962807</t>
+  </si>
+  <si>
+    <t>-82.940886</t>
+  </si>
+  <si>
+    <t>-82.966426</t>
+  </si>
+  <si>
+    <t>-82.929915</t>
+  </si>
+  <si>
+    <t>-82.920525</t>
+  </si>
+  <si>
+    <t>-82.944537</t>
+  </si>
+  <si>
+    <t>-82.964993</t>
+  </si>
+  <si>
+    <t>-82.924711</t>
+  </si>
+  <si>
+    <t>-82.934028</t>
+  </si>
+  <si>
+    <t>-82.958903</t>
+  </si>
+  <si>
+    <t>-82.952741</t>
+  </si>
+  <si>
+    <t>-82.918491</t>
+  </si>
+  <si>
+    <t>-82.958237</t>
+  </si>
+  <si>
+    <t>42.479976</t>
+  </si>
+  <si>
+    <t>42.479825</t>
+  </si>
+  <si>
+    <t>42.479803</t>
+  </si>
+  <si>
+    <t>42.465404</t>
+  </si>
+  <si>
+    <t>42.479923</t>
+  </si>
+  <si>
+    <t>42.459181</t>
+  </si>
+  <si>
+    <t>42.479876</t>
+  </si>
+  <si>
+    <t>-82.964470</t>
+  </si>
+  <si>
+    <t>-82.937518</t>
+  </si>
+  <si>
+    <t>-82.955558</t>
+  </si>
+  <si>
+    <t>-82.961050</t>
+  </si>
+  <si>
+    <t>-82.956645</t>
+  </si>
+  <si>
+    <t>-82.938276</t>
+  </si>
+  <si>
+    <t>-82.931126</t>
+  </si>
+  <si>
+    <t>-82.928295</t>
+  </si>
+  <si>
+    <t>-82.955936</t>
+  </si>
+  <si>
+    <t>-82.948824</t>
+  </si>
+  <si>
+    <t>-82.960984</t>
+  </si>
+  <si>
+    <t>-82.932982</t>
+  </si>
+  <si>
+    <t>-82.929948</t>
+  </si>
+  <si>
+    <t>-82.960277</t>
+  </si>
+  <si>
+    <t>-82.938304</t>
+  </si>
+  <si>
+    <t>-82.942593</t>
+  </si>
+  <si>
+    <t>-82.934832</t>
+  </si>
+  <si>
+    <t>-82.963968</t>
+  </si>
+  <si>
+    <t>-82.968444</t>
+  </si>
+  <si>
+    <t>-82.937006</t>
+  </si>
+  <si>
+    <t>42.453855</t>
+  </si>
+  <si>
+    <t>42.465058</t>
+  </si>
+  <si>
+    <t>42.465148</t>
+  </si>
+  <si>
+    <t>42.480226</t>
+  </si>
+  <si>
+    <t>42.479489</t>
+  </si>
+  <si>
+    <t>42.460782</t>
+  </si>
+  <si>
+    <t>42.459500</t>
+  </si>
+  <si>
+    <t>42.465146</t>
+  </si>
+  <si>
+    <t>42.463094</t>
+  </si>
+  <si>
+    <t>42.465354</t>
+  </si>
+  <si>
+    <t>42.450736</t>
+  </si>
+  <si>
+    <t>42.465537</t>
+  </si>
+  <si>
+    <t>42.456441</t>
+  </si>
+  <si>
+    <t>42.450380</t>
+  </si>
+  <si>
+    <t>42.465453</t>
+  </si>
+  <si>
+    <t>-82.960226</t>
+  </si>
+  <si>
+    <t>-82.943988</t>
+  </si>
+  <si>
+    <t>-82.935152</t>
+  </si>
+  <si>
+    <t>-82.932341</t>
+  </si>
+  <si>
+    <t>-82.924976</t>
+  </si>
+  <si>
+    <t>42.463214</t>
+  </si>
+  <si>
+    <t>42.465341</t>
+  </si>
+  <si>
+    <t>42.464982</t>
+  </si>
+  <si>
+    <t>42.465000</t>
+  </si>
+  <si>
+    <t>42.465315</t>
+  </si>
+  <si>
+    <t>-82.949271</t>
+  </si>
+  <si>
+    <t>-82.941100</t>
+  </si>
+  <si>
+    <t>-82.940718</t>
+  </si>
+  <si>
+    <t>-82.967218</t>
+  </si>
+  <si>
+    <t>42.480257</t>
+  </si>
+  <si>
+    <t>42.464771</t>
+  </si>
+  <si>
+    <t>42.464743</t>
+  </si>
+  <si>
+    <t>42.472294</t>
   </si>
 </sst>
 </file>
@@ -591,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -606,6 +783,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -889,32 +1069,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="97.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="4"/>
+    <col min="3" max="3" width="26.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>16</v>
@@ -929,31 +1110,34 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="str">
-        <f>CONCATENATE("y[",ROW()-2,"] = [",B2,", '",C2,"', '",D2,"', '",E2,"', g(",F2,"), ",G2,", '",K2,"'];")</f>
-        <v>y[0] = [1, 'Cloverleaf Bar &amp; Restaurant', '', '24443 Gratiot Avenue', g(42.474663, -82.952055), 1, 'Alcohol, American, Bar, Pizza'];</v>
+        <f>CONCATENATE("y[",ROW()-2,"] = [",B2,", '",C2,"', '",D2,"', '",E2,"', ",F2,", ",G2,", ",H2,", '",L2,"'];")</f>
+        <v>y[0] = [1, 'Cloverleaf Bar &amp; Restaurant', '', '24443 Gratiot Avenue', 42.474663, -82.952055, 1, 'Alcohol, American, Bar, Pizza'];</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -965,10 +1149,10 @@
         <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
@@ -977,19 +1161,22 @@
         <v>1</v>
       </c>
       <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>169</v>
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
-        <f t="shared" ref="A3:A65" si="0">CONCATENATE("y[",ROW()-2,"] = [",B3,", '",C3,"', '",D3,"', '",E3,"', g(",F3,"), ",G3,", '",K3,"'];")</f>
-        <v>y[1] = [1, 'Villa Restaurant &amp; Pizzeria', '', '21311 Gratiot Avenue', g(42.454643, -82.965264), 1, 'Italian, Pizza'];</v>
+        <f t="shared" ref="A3:A65" si="0">CONCATENATE("y[",ROW()-2,"] = [",B3,", '",C3,"', '",D3,"', '",E3,"', ",F3,", ",G3,", ",H3,", '",L3,"'];")</f>
+        <v>y[1] = [1, 'Villa Restaurant &amp; Pizzeria', '', '21311 Gratiot Avenue', 42.454643, -82.965264, 1, 'Italian, Pizza'];</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -1001,49 +1188,55 @@
         <v>63</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>170</v>
+        <v>115</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[2] = [1, 'Donna&amp;apos;s Family Dining', '', '18640 East 10 Mile Road', g(42.479889, -82.927846), 1, 'American, Diner'];</v>
+        <v>y[2] = [1, 'Donna&amp;apos;s Family Dining', '', '18640 East 10 Mile Road', 42.479889, -82.927846, 1, 'American, Diner'];</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[3] = [1, 'Friends Tavern', '', '23850 Gratiot Avenue', g(42.472043, -82.952674), 1, 'Bar'];</v>
+        <v>y[3] = [1, 'Friends Tavern', '', '23850 Gratiot Avenue', 42.472043, -82.952674, 1, 'Bar'];</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -1055,106 +1248,118 @@
         <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[4] = [1, 'Grand Dimitre&amp;apos;s', '', '25001 Gratiot Avenue', g(42.480217, -82.948572), 1, 'Diner, American'];</v>
+        <v>y[4] = [1, 'Grand Dimitre&amp;apos;s', '', '25001 Gratiot Avenue', 42.480217, -82.948572, 1, 'Diner, American'];</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[5] = [1, 'Hungry Howie&amp;apos;s Pizza', '', '22441 Kelly Road', g(42.463503, -82.928942), 1, 'Pizza'];</v>
+        <v>y[5] = [1, 'Hungry Howie&amp;apos;s Pizza', '', '22441 Kelly Road', 42.463503, -82.928942, 1, 'Pizza'];</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>7</v>
+        <v>119</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[6] = [1, 'McDonald&amp;apos;s', '', '17921 East 9 Mile Road', g(42.465577, -82.935909), 1, 'American'];</v>
+        <v>y[6] = [1, 'McDonald&amp;apos;s', '', '17921 East 9 Mile Road', 42.465577, -82.935909, 1, 'American'];</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>165</v>
+        <v>105</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[7] = [1, 'Olive Garden', '', '24845 Gratiot Avenue', g(42.478462, -82.949634), 1, 'Italian'];</v>
+        <v>y[7] = [1, 'Olive Garden', '', '24845 Gratiot Avenue', 42.478462, -82.949634, 1, 'Italian'];</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -1166,73 +1371,82 @@
         <v>67</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[8] = [1, 'Papa John&amp;apos;s Pizza', '', '22241 Kelly Road', g(42.462028, -82.930547), 1, 'Pizza'];</v>
+        <v>y[8] = [1, 'Papa John&amp;apos;s Pizza', '', '22241 Kelly Road', 42.462028, -82.930547, 1, 'Pizza'];</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>164</v>
+        <v>104</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="K10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[9] = [1, 'Papa Romano&amp;apos;s &amp; Mr. Pita', '', '22661 Gratiot Avenue', g(42.464322, -82.959707), 1, 'Pizza'];</v>
+        <v>y[9] = [1, 'Papa Romano&amp;apos;s &amp; Mr. Pita', '', '22661 Gratiot Avenue', 42.464322, -82.959707, 1, 'Pizza'];</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="K11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[10] = [1, 'Pizza Me', '', '', g(), 1, 'Pizza'];</v>
+        <v>y[10] = [1, 'Pizza Me', '', '', , , 1, 'Pizza'];</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
@@ -1240,20 +1454,20 @@
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[11] = [1, 'Salvatore Scallopini', '', '22611 Gratiot Avenue', g(42.463848, -82.959658), 1, 'Italian'];</v>
+        <v>y[11] = [1, 'Salvatore Scallopini', '', '22611 Gratiot Avenue', 42.463848, -82.959658, 1, 'Italian'];</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
@@ -1262,25 +1476,28 @@
         <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[12] = [1, 'Sugarbush Tavern', '', '19080 East 10 Mile Road', g(42.479991, -82.921896), 1, 'Bar, American'];</v>
+        <v>y[12] = [1, 'Sugarbush Tavern', '', '19080 East 10 Mile Road', 42.479991, -82.921896, 1, 'Bar, American'];</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
@@ -1289,52 +1506,58 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[13] = [1, 'Tim Horton&amp;apos;s', '', '17210 East 9 Mile Road', g(42.464667, -82.944054), 1, 'Coffee'];</v>
+        <v>y[13] = [1, 'Tim Horton&amp;apos;s', '', '17210 East 9 Mile Road', 42.464667, -82.944054, 1, 'Coffee'];</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>162</v>
+        <v>102</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="4">
-        <v>1</v>
-      </c>
-      <c r="K15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[14] = [1, '10x Better Soul Food', '', '', g(), 0, 'BBQ'];</v>
+        <v>y[14] = [1, '10x Better Soul Food', '', '', , , 0, 'BBQ'];</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -1342,65 +1565,71 @@
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
       <c r="H16" s="4">
         <v>0</v>
       </c>
       <c r="I16" s="4">
-        <v>1</v>
-      </c>
-      <c r="K16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[15] = [1, 'Adriana&amp;apos;s Kitchen', '', '', g(42.465112, -82.948927), 0, ''];</v>
+        <v>y[15] = [1, 'Adriana&amp;apos;s Kitchen', '', '', 42.465112, -82.948927, 0, ''];</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[16] = [1, 'Andary&amp;apos;s Grill &amp; Deli', '', '', g(42.470411, -82.954819), 0, ''];</v>
+        <v>y[16] = [1, 'Andary&amp;apos;s Grill &amp; Deli', '', '', 42.470411, -82.954819, 0, ''];</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[17] = [1, 'Big Boy', '', '', g(42.465559, -82.958383), 0, ''];</v>
+        <v>y[17] = [1, 'Big Boy', '', '', 42.465559, -82.958383, 0, ''];</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
@@ -1409,19 +1638,22 @@
         <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
-      <c r="L19" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[18] = [1, 'Boney Moroney Bar', '', '', g(42.456316, -82.962807), 0, ''];</v>
+        <v>y[18] = [1, 'Boney Moroney Bar', '', '', 42.456316, -82.962807, 0, ''];</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
@@ -1430,16 +1662,19 @@
         <v>18</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[19] = [1, 'Bread Basket Deli', '', '', g(42.450935, -82.940886), 0, ''];</v>
+        <v>y[19] = [1, 'Bread Basket Deli', '', '', 42.450935, -82.940886, 0, ''];</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
@@ -1448,16 +1683,19 @@
         <v>19</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[20] = [1, 'Burger King', '', '', g(42.450942, -82.966426), 0, ''];</v>
+        <v>y[20] = [1, 'Burger King', '', '', 42.450942, -82.966426, 0, ''];</v>
       </c>
       <c r="B22" s="4">
         <v>1</v>
@@ -1466,16 +1704,19 @@
         <v>20</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[21] = [1, 'China Wok', '', '', g(42.462667, -82.929915), 0, ''];</v>
+        <v>y[21] = [1, 'China Wok', '', '', 42.462667, -82.929915, 0, ''];</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
@@ -1484,16 +1725,19 @@
         <v>21</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[22] = [1, 'Coffee Break Café', '', '', g(42.479804, -82.920525), 0, ''];</v>
+        <v>y[22] = [1, 'Coffee Break Café', '', '', 42.479804, -82.920525, 0, ''];</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -1502,55 +1746,64 @@
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[23] = [1, 'Dairy Queen Brazier', '', '', g(42.465111, -82.944537), 0, ''];</v>
+        <v>y[23] = [1, 'Dairy Queen Brazier', '', '', 42.465111, -82.944537, 0, ''];</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G25" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[24] = [1, 'Domino&amp;apos;s Pizza', '', '', g(42.479924, -82.964993), 0, 'Pizza'];</v>
+        <v>y[24] = [1, 'Domino&amp;apos;s Pizza', '', '', 42.479924, -82.964993, 0, 'Pizza'];</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>159</v>
+        <v>99</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="4">
-        <v>0</v>
-      </c>
-      <c r="K26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[25] = [1, 'Eastpointe Pub', '', '', g(42.465298, -82.924711), 0, ''];</v>
+        <v>y[25] = [1, 'Eastpointe Pub', '', '', 42.465298, -82.924711, 0, ''];</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
@@ -1559,16 +1812,19 @@
         <v>23</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[26] = [1, 'Five Guys &amp; Fries', '', '', g(42.464157, -82.959707), 0, ''];</v>
+        <v>y[26] = [1, 'Five Guys &amp; Fries', '', '', 42.464157, -82.959707, 0, ''];</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
@@ -1577,34 +1833,40 @@
         <v>24</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[27] = [1, 'Guiseppe&amp;apos;s Bakery', '', '', g(42.458315, -82.934028), 0, ''];</v>
+        <v>y[27] = [1, 'Guiseppe&amp;apos;s Bakery', '', '', 42.458315, -82.934028, 0, ''];</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G29" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[28] = [1, 'Happy Garden', '', '', g(42.462424, -82.958903), 0, ''];</v>
+        <v>y[28] = [1, 'Happy Garden', '', '', 42.462424, -82.958903, 0, ''];</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
@@ -1613,172 +1875,199 @@
         <v>25</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G30" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[29] = [1, 'Happy&amp;apos;s Pizza', '', '', g(42.471669, -82.952741), 0, 'Pizza'];</v>
+        <v>y[29] = [1, 'Happy&amp;apos;s Pizza', '', '', 42.471669, -82.952741, 0, 'Pizza'];</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" s="4">
-        <v>0</v>
-      </c>
-      <c r="K31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[30] = [1, 'Jet&amp;apos;s Pizza', '', '', g(42.479976, -82.918491), 0, 'Pizza'];</v>
+        <v>y[30] = [1, 'Jet&amp;apos;s Pizza', '', '', 42.479976, -82.918491, 0, 'Pizza'];</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" s="4">
-        <v>0</v>
-      </c>
-      <c r="K32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[31] = [1, 'KC&amp;apos;s Dairy Twist', '', '', g(42.479825, -82.958237), 0, ''];</v>
+        <v>y[31] = [1, 'KC&amp;apos;s Dairy Twist', '', '', 42.479825, -82.958237, 0, ''];</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[32] = [1, 'Marz Bar', '', '', g(42.479803, -82.964470), 0, ''];</v>
+        <v>y[32] = [1, 'Marz Bar', '', '', 42.479803, -82.964470, 0, ''];</v>
       </c>
       <c r="B34" s="4">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G34" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[33] = [1, 'Legend&amp;apos;s Coney Express', '', '', g(42.465404, -82.937518), 0, ''];</v>
+        <v>y[33] = [1, 'Legend&amp;apos;s Coney Express', '', '', 42.465404, -82.937518, 0, ''];</v>
       </c>
       <c r="B35" s="4">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G35" s="4">
-        <v>0</v>
-      </c>
-      <c r="J35" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[34] = [1, 'Little Caesar&amp;apos;s', '', '', g(42.479923, -82.955558), 0, 'Pizza'];</v>
+        <v>y[34] = [1, 'Little Caesar&amp;apos;s', '', '', 42.479923, -82.955558, 0, 'Pizza'];</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G36" s="4">
-        <v>0</v>
-      </c>
-      <c r="K36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[35] = [1, 'McGee&amp;apos;s Lounge', '', '', g(42.459181, -82.961050), 0, ''];</v>
+        <v>y[35] = [1, 'McGee&amp;apos;s Lounge', '', '', 42.459181, -82.961050, 0, ''];</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G37" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[36] = [1, 'O&amp;apos;Hara&amp;apos;s Irish Pub', '', '', g(42.479876, -82.956645), 0, ''];</v>
+        <v>y[36] = [1, 'O&amp;apos;Hara&amp;apos;s Irish Pub', '', '', 42.479876, -82.956645, 0, ''];</v>
       </c>
       <c r="B38" s="4">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G38" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[37] = [1, 'Panda', '', '', g(), 0, ''];</v>
+        <v>y[37] = [1, 'Panda', '', '', , , 0, ''];</v>
       </c>
       <c r="B39" s="4">
         <v>1</v>
@@ -1786,14 +2075,14 @@
       <c r="C39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G39" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[38] = [1, 'Pizza Square', '', '', g(42.453855, -82.938276), 0, 'Pizza'];</v>
+        <v>y[38] = [1, 'Pizza Square', '', '', 42.453855, -82.938276, 0, 'Pizza'];</v>
       </c>
       <c r="B40" s="4">
         <v>1</v>
@@ -1802,19 +2091,22 @@
         <v>27</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G40" s="4">
-        <v>0</v>
-      </c>
-      <c r="K40" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[39] = [1, 'Plaza Mexico', '', '', g(42.465058, -82.931126), 0, ''];</v>
+        <v>y[39] = [1, 'Plaza Mexico', '', '', 42.465058, -82.931126, 0, ''];</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
@@ -1823,34 +2115,40 @@
         <v>28</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G41" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[40] = [1, 'Popeye&amp;apos;s', '', '', g(42.465148, -82.928295), 0, ''];</v>
+        <v>y[40] = [1, 'Popeye&amp;apos;s', '', '', 42.465148, -82.928295, 0, ''];</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G42" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[41] = [1, 'Scoreboard Sports Bar &amp; Grill', '', '', g(42.480226, -82.955936), 0, ''];</v>
+        <v>y[41] = [1, 'Scoreboard Sports Bar &amp; Grill', '', '', 42.480226, -82.955936, 0, ''];</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
@@ -1859,16 +2157,19 @@
         <v>29</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G43" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[42] = [1, 'Shawarma Express', '', '', g(42.479489, -82.948824), 0, ''];</v>
+        <v>y[42] = [1, 'Shawarma Express', '', '', 42.479489, -82.948824, 0, ''];</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
@@ -1877,16 +2178,19 @@
         <v>30</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G44" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[43] = [1, 'Shish Kabob', '', '', g(42.460782, -82.960984), 0, ''];</v>
+        <v>y[43] = [1, 'Shish Kabob', '', '', 42.460782, -82.960984, 0, ''];</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
@@ -1895,34 +2199,40 @@
         <v>31</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G45" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[44] = [1, 'Snooker&amp;apos;s Pool &amp; Pub', '', '', g(42.459500, -82.932982), 0, ''];</v>
+        <v>y[44] = [1, 'Snooker&amp;apos;s Pool &amp; Pub', '', '', 42.459500, -82.932982, 0, ''];</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G46" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[45] = [1, 'Subway', '', '', g(42.465146, -82.929948), 0, ''];</v>
+        <v>y[45] = [1, 'Subway', '', '', 42.465146, -82.929948, 0, ''];</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
@@ -1931,16 +2241,19 @@
         <v>32</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G47" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[46] = [1, 'Subway', '', '', g(42.463094, -82.960277), 0, ''];</v>
+        <v>y[46] = [1, 'Subway', '', '', 42.463094, -82.960277, 0, ''];</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -1949,16 +2262,19 @@
         <v>32</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G48" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[47] = [1, 'Taco Bell', '', '', g(42.465354, -82.938304), 0, ''];</v>
+        <v>y[47] = [1, 'Taco Bell', '', '', 42.465354, -82.938304, 0, ''];</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
@@ -1967,16 +2283,19 @@
         <v>33</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G49" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[48] = [1, 'Wah Hong Chop Suey', '', '', g(42.450736, -82.942593), 0, ''];</v>
+        <v>y[48] = [1, 'Wah Hong Chop Suey', '', '', 42.450736, -82.942593, 0, ''];</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -1985,34 +2304,40 @@
         <v>34</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G50" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[49] = [1, 'Wendy&amp;apos;s', '', '', g(42.465537, -82.934832), 0, ''];</v>
+        <v>y[49] = [1, 'Wendy&amp;apos;s', '', '', 42.465537, -82.934832, 0, ''];</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G51" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H51" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[50] = [1, 'Western', '', '', g(42.456441, -82.963968), 0, ''];</v>
+        <v>y[50] = [1, 'Western', '', '', 42.456441, -82.963968, 0, ''];</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
@@ -2021,16 +2346,19 @@
         <v>35</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G52" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H52" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[51] = [1, 'White Castle', '', '', g(42.450380, -82.968444), 0, ''];</v>
+        <v>y[51] = [1, 'White Castle', '', '', 42.450380, -82.968444, 0, ''];</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
@@ -2039,16 +2367,19 @@
         <v>36</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G53" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H53" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[52] = [1, 'Milestone Grill', '', '', g(42.465453, -82.937006), 0, 'Pizza'];</v>
+        <v>y[52] = [1, 'Milestone Grill', '', '', 42.465453, -82.937006, 0, 'Pizza'];</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -2057,34 +2388,37 @@
         <v>47</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G54" s="4">
-        <v>0</v>
-      </c>
-      <c r="K54" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H54" s="4">
+        <v>0</v>
+      </c>
+      <c r="L54" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[53] = [1, 'Ashby&amp;apos;s', '', '', g(), 0, ''];</v>
+        <v>y[53] = [1, 'Ashby&amp;apos;s', '', '', , , 0, ''];</v>
       </c>
       <c r="B55" s="4">
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G55" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="H55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[54] = [1, 'Wing Stop', '', '', g(42.463214, -82.960226), 0, ''];</v>
+        <v>y[54] = [1, 'Wing Stop', '', '', 42.463214, -82.960226, 0, ''];</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
@@ -2093,70 +2427,82 @@
         <v>48</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G56" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[55] = [1, 'Granma&amp;apos;s House of Pancakes', '', '', g(42.465341, -82.943988), 0, ''];</v>
+        <v>y[55] = [1, 'Granma&amp;apos;s House of Pancakes', '', '', 42.465341, -82.943988, 0, ''];</v>
       </c>
       <c r="B57" s="4">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>146</v>
+        <v>86</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G57" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H57" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[56] = [1, 'Josephine&amp;apos;s Soul Food', '', '', g(42.464982, -82.935152), 0, ''];</v>
+        <v>y[56] = [1, 'Josephine&amp;apos;s Soul Food', '', '', 42.464982, -82.935152, 0, ''];</v>
       </c>
       <c r="B58" s="4">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G58" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H58" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[57] = [1, 'Sullivan&amp;apos;s', '', '', g(42.465000, -82.932341), 0, ''];</v>
+        <v>y[57] = [1, 'Sullivan&amp;apos;s', '', '', 42.465000, -82.932341, 0, ''];</v>
       </c>
       <c r="B59" s="4">
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G59" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H59" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[58] = [1, 'Di Frattelli Pizza', '', '', g(42.465315, -82.924976), 0, 'Pizza'];</v>
+        <v>y[58] = [1, 'Di Frattelli Pizza', '', '', 42.465315, -82.924976, 0, 'Pizza'];</v>
       </c>
       <c r="B60" s="4">
         <v>1</v>
@@ -2165,19 +2511,22 @@
         <v>49</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G60" s="4">
-        <v>0</v>
-      </c>
-      <c r="K60" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H60" s="4">
+        <v>0</v>
+      </c>
+      <c r="L60" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[59] = [1, 'Gratiot Avenue Memory Lane Café', '', '', g(), 0, ''];</v>
+        <v>y[59] = [1, 'Gratiot Avenue Memory Lane Café', '', '', , , 0, ''];</v>
       </c>
       <c r="B61" s="4">
         <v>1</v>
@@ -2185,14 +2534,14 @@
       <c r="C61" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G61" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H61" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[60] = [1, 'Passport Pizza', '', '', g(42.480257, -82.949271), 0, 'Pizza'];</v>
+        <v>y[60] = [1, 'Passport Pizza', '', '', 42.480257, -82.949271, 0, 'Pizza'];</v>
       </c>
       <c r="B62" s="4">
         <v>1</v>
@@ -2201,85 +2550,99 @@
         <v>51</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G62" s="4">
-        <v>0</v>
-      </c>
-      <c r="K62" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H62" s="4">
+        <v>0</v>
+      </c>
+      <c r="L62" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[61] = [1, 'East Detroit Bakery', '', '', g(42.464771, -82.941100), 0, ''];</v>
+        <v>y[61] = [1, 'East Detroit Bakery', '', '', 42.464771, -82.941100, 0, ''];</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[62] = [1, 'Cup Cakes &amp; Ice Cream Kids', '', '', g(42.464743, -82.940718), 0, ''];</v>
+        <v>y[62] = [1, 'Cup Cakes &amp; Ice Cream Kids', '', '', 42.464743, -82.940718, 0, ''];</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[63] = [1, 'Taormina&amp;apos;s Pizza &amp; Ice Cream', '', '', g(42.472294, -82.967218), 0, 'Pizza'];</v>
+        <v>y[63] = [1, 'Taormina&amp;apos;s Pizza &amp; Ice Cream', '', '', 42.472294, -82.967218, 0, 'Pizza'];</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K65" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L65" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C67" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
     </row>
   </sheetData>
-  <sortState ref="L2:L12">
-    <sortCondition ref="L2"/>
+  <sortState ref="M2:M12">
+    <sortCondition ref="M2"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="C67:E67"/>

</xml_diff>

<commit_message>
Added more comprehensive types
</commit_message>
<xml_diff>
--- a/EATSpointe.xlsx
+++ b/EATSpointe.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="246">
   <si>
     <t>Restaurant</t>
   </si>
@@ -194,18 +194,9 @@
     <t>Diner</t>
   </si>
   <si>
-    <t>American, Diner</t>
-  </si>
-  <si>
-    <t>Diner, American</t>
-  </si>
-  <si>
     <t>Sandwiches</t>
   </si>
   <si>
-    <t>Bar, American</t>
-  </si>
-  <si>
     <t>BBQ</t>
   </si>
   <si>
@@ -353,12 +344,6 @@
     <t>Donna&amp;apos;s Family Dining</t>
   </si>
   <si>
-    <t>Alcohol, American, Bar, Pizza</t>
-  </si>
-  <si>
-    <t>Italian, Pizza</t>
-  </si>
-  <si>
     <t>CODE</t>
   </si>
   <si>
@@ -717,6 +702,66 @@
   </si>
   <si>
     <t>42.472294</t>
+  </si>
+  <si>
+    <t>Alcohol, American, Bar, Pizza, Italian, Sandwiches, Family friendly</t>
+  </si>
+  <si>
+    <t>Italian, Pizza, Alcohol, Family friendly</t>
+  </si>
+  <si>
+    <t>American, Diner, Sandwiches, Coffee</t>
+  </si>
+  <si>
+    <t>Bar, Alcohol</t>
+  </si>
+  <si>
+    <t>American, Coffee</t>
+  </si>
+  <si>
+    <t>Italian, Alcohol</t>
+  </si>
+  <si>
+    <t>Bar, American, Sandwiches</t>
+  </si>
+  <si>
+    <t>American, Coffee, Family friendly</t>
+  </si>
+  <si>
+    <t>American, Sandwiches, Coffee</t>
+  </si>
+  <si>
+    <t>Ice Cream</t>
+  </si>
+  <si>
+    <t>American, Sandwiches, Family friendly, Ice Cream</t>
+  </si>
+  <si>
+    <t>Ice Cream, Family friendly</t>
+  </si>
+  <si>
+    <t>American, Sandwiches</t>
+  </si>
+  <si>
+    <t>American, Sandwiches, Alcohol</t>
+  </si>
+  <si>
+    <t>Mediterranean</t>
+  </si>
+  <si>
+    <t>Bar, Alcohol, American</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Pizza, Bar, Alcohol, Mediterranean</t>
+  </si>
+  <si>
+    <t>American, Breakfast</t>
+  </si>
+  <si>
+    <t>Diner, American, Coffee, Breakfast</t>
   </si>
 </sst>
 </file>
@@ -1071,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,14 +1133,14 @@
     <col min="9" max="9" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="56.44140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="19.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>16</v>
@@ -1110,10 +1155,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
@@ -1137,7 +1182,7 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="str">
         <f>CONCATENATE("y[",ROW()-2,"] = [",B2,", '",C2,"', '",D2,"', '",E2,"', ",F2,", ",G2,", ",H2,", '",L2,"'];")</f>
-        <v>y[0] = [1, 'Cloverleaf Bar &amp; Restaurant', '', '24443 Gratiot Avenue', 42.474663, -82.952055, 1, 'Alcohol, American, Bar, Pizza'];</v>
+        <v>y[0] = [1, 'Cloverleaf Bar &amp; Restaurant', '', '24443 Gratiot Avenue', 42.474663, -82.952055, 1, 'Alcohol, American, Bar, Pizza, Italian, Sandwiches, Family friendly'];</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1146,13 +1191,13 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
@@ -1167,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>109</v>
+        <v>226</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>38</v>
@@ -1176,58 +1221,58 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f t="shared" ref="A3:A65" si="0">CONCATENATE("y[",ROW()-2,"] = [",B3,", '",C3,"', '",D3,"', '",E3,"', ",F3,", ",G3,", ",H3,", '",L3,"'];")</f>
-        <v>y[1] = [1, 'Villa Restaurant &amp; Pizzeria', '', '21311 Gratiot Avenue', 42.454643, -82.965264, 1, 'Italian, Pizza'];</v>
+        <v>y[1] = [1, 'Villa Restaurant &amp; Pizzeria', '', '21311 Gratiot Avenue', 42.454643, -82.965264, 1, 'Italian, Pizza, Alcohol, Family friendly'];</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H3" s="4">
         <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>110</v>
+        <v>227</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[2] = [1, 'Donna&amp;apos;s Family Dining', '', '18640 East 10 Mile Road', 42.479889, -82.927846, 1, 'American, Diner'];</v>
+        <v>y[2] = [1, 'Donna&amp;apos;s Family Dining', '', '18640 East 10 Mile Road', 42.479889, -82.927846, 1, 'American, Diner, Sandwiches, Coffee'];</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>56</v>
+        <v>228</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>40</v>
@@ -1236,7 +1281,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[3] = [1, 'Friends Tavern', '', '23850 Gratiot Avenue', 42.472043, -82.952674, 1, 'Bar'];</v>
+        <v>y[3] = [1, 'Friends Tavern', '', '23850 Gratiot Avenue', 42.472043, -82.952674, 1, 'Bar, Alcohol'];</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -1245,19 +1290,19 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H5" s="4">
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>46</v>
+        <v>229</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>8</v>
@@ -1266,31 +1311,31 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[4] = [1, 'Grand Dimitre&amp;apos;s', '', '25001 Gratiot Avenue', 42.480217, -82.948572, 1, 'Diner, American'];</v>
+        <v>y[4] = [1, 'Grand Dimitre&amp;apos;s', '', '25001 Gratiot Avenue', 42.480217, -82.948572, 1, 'Diner, American, Coffee, Breakfast'];</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>57</v>
+        <v>245</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1302,16 +1347,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H7" s="4">
         <v>1</v>
@@ -1320,28 +1365,28 @@
         <v>7</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[6] = [1, 'McDonald&amp;apos;s', '', '17921 East 9 Mile Road', 42.465577, -82.935909, 1, 'American'];</v>
+        <v>y[6] = [1, 'McDonald&amp;apos;s', '', '17921 East 9 Mile Road', 42.465577, -82.935909, 1, 'American, Coffee'];</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H8" s="4">
         <v>1</v>
@@ -1350,16 +1395,16 @@
         <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>58</v>
+        <v>230</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[7] = [1, 'Olive Garden', '', '24845 Gratiot Avenue', 42.478462, -82.949634, 1, 'Italian'];</v>
+        <v>y[7] = [1, 'Olive Garden', '', '24845 Gratiot Avenue', 42.478462, -82.949634, 1, 'Italian, Alcohol'];</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -1368,19 +1413,22 @@
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H9" s="4">
         <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>8</v>
+        <v>231</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1392,16 +1440,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
@@ -1409,9 +1457,6 @@
       <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
@@ -1422,16 +1467,16 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H11" s="4">
         <v>1</v>
@@ -1440,7 +1485,7 @@
         <v>7</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1461,13 +1506,13 @@
         <v>7</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[11] = [1, 'Salvatore Scallopini', '', '22611 Gratiot Avenue', 42.463848, -82.959658, 1, 'Italian'];</v>
+        <v>y[11] = [1, 'Salvatore Scallopini', '', '22611 Gratiot Avenue', 42.463848, -82.959658, 1, 'Italian, Alcohol'];</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
@@ -1476,28 +1521,28 @@
         <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H13" s="4">
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>8</v>
+        <v>231</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[12] = [1, 'Sugarbush Tavern', '', '19080 East 10 Mile Road', 42.479991, -82.921896, 1, 'Bar, American'];</v>
+        <v>y[12] = [1, 'Sugarbush Tavern', '', '19080 East 10 Mile Road', 42.479991, -82.921896, 1, 'Bar, American, Sandwiches'];</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
@@ -1506,22 +1551,22 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H14" s="4">
         <v>1</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>55</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1533,16 +1578,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="H15" s="4">
         <v>1</v>
@@ -1551,7 +1596,7 @@
         <v>39</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1575,61 +1620,70 @@
         <v>1</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[15] = [1, 'Adriana&amp;apos;s Kitchen', '', '', 42.465112, -82.948927, 0, ''];</v>
+        <v>y[15] = [1, 'Adriana&amp;apos;s Kitchen', '', '', 42.465112, -82.948927, 0, 'American'];</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H17" s="4">
         <v>0</v>
       </c>
+      <c r="L17" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="M17" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[16] = [1, 'Andary&amp;apos;s Grill &amp; Deli', '', '', 42.470411, -82.954819, 0, ''];</v>
+        <v>y[16] = [1, 'Andary&amp;apos;s Grill &amp; Deli', '', '', 42.470411, -82.954819, 0, 'American, Coffee, Family friendly'];</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H18" s="4">
         <v>0</v>
       </c>
+      <c r="L18" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="M18" s="1" t="s">
-        <v>42</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[17] = [1, 'Big Boy', '', '', 42.465559, -82.958383, 0, ''];</v>
+        <v>y[17] = [1, 'Big Boy', '', '', 42.465559, -82.958383, 0, 'American, Sandwiches, Coffee'];</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
@@ -1638,22 +1692,22 @@
         <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H19" s="4">
         <v>0</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>43</v>
+      <c r="L19" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[18] = [1, 'Boney Moroney Bar', '', '', 42.456316, -82.962807, 0, ''];</v>
+        <v>y[18] = [1, 'Boney Moroney Bar', '', '', 42.456316, -82.962807, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
@@ -1662,19 +1716,25 @@
         <v>18</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H20" s="4">
         <v>0</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[19] = [1, 'Bread Basket Deli', '', '', 42.450935, -82.940886, 0, ''];</v>
+        <v>y[19] = [1, 'Bread Basket Deli', '', '', 42.450935, -82.940886, 0, 'Sandwiches'];</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
@@ -1683,19 +1743,25 @@
         <v>19</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H21" s="4">
         <v>0</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[20] = [1, 'Burger King', '', '', 42.450942, -82.966426, 0, ''];</v>
+        <v>y[20] = [1, 'Burger King', '', '', 42.450942, -82.966426, 0, 'Sandwiches'];</v>
       </c>
       <c r="B22" s="4">
         <v>1</v>
@@ -1704,19 +1770,25 @@
         <v>20</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H22" s="4">
         <v>0</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[21] = [1, 'China Wok', '', '', 42.462667, -82.929915, 0, ''];</v>
+        <v>y[21] = [1, 'China Wok', '', '', 42.462667, -82.929915, 0, 'Chinese'];</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
@@ -1725,19 +1797,22 @@
         <v>21</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H23" s="4">
         <v>0</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[22] = [1, 'Coffee Break Café', '', '', 42.479804, -82.920525, 0, ''];</v>
+        <v>y[22] = [1, 'Coffee Break Café', '', '', 42.479804, -82.920525, 0, 'Coffee'];</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -1746,34 +1821,40 @@
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H24" s="4">
         <v>0</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[23] = [1, 'Dairy Queen Brazier', '', '', 42.465111, -82.944537, 0, ''];</v>
+        <v>y[23] = [1, 'Dairy Queen Brazier', '', '', 42.465111, -82.944537, 0, 'American, Sandwiches, Family friendly, Ice Cream'];</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H25" s="4">
         <v>0</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1785,13 +1866,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H26" s="4">
         <v>0</v>
@@ -1803,7 +1884,7 @@
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[25] = [1, 'Eastpointe Pub', '', '', 42.465298, -82.924711, 0, ''];</v>
+        <v>y[25] = [1, 'Eastpointe Pub', '', '', 42.465298, -82.924711, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
@@ -1812,19 +1893,22 @@
         <v>23</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H27" s="4">
         <v>0</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[26] = [1, 'Five Guys &amp; Fries', '', '', 42.464157, -82.959707, 0, ''];</v>
+        <v>y[26] = [1, 'Five Guys &amp; Fries', '', '', 42.464157, -82.959707, 0, 'Sandwiches'];</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
@@ -1833,40 +1917,46 @@
         <v>24</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H28" s="4">
         <v>0</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[27] = [1, 'Guiseppe&amp;apos;s Bakery', '', '', 42.458315, -82.934028, 0, ''];</v>
+        <v>y[27] = [1, 'Guiseppe&amp;apos;s Bakery', '', '', 42.458315, -82.934028, 0, 'Bakery'];</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H29" s="4">
         <v>0</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[28] = [1, 'Happy Garden', '', '', 42.462424, -82.958903, 0, ''];</v>
+        <v>y[28] = [1, 'Happy Garden', '', '', 42.462424, -82.958903, 0, 'Chinese'];</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
@@ -1875,13 +1965,16 @@
         <v>25</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H30" s="4">
         <v>0</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -1893,13 +1986,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H31" s="4">
         <v>0</v>
@@ -1917,13 +2010,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H32" s="4">
         <v>0</v>
@@ -1935,67 +2028,76 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[31] = [1, 'KC&amp;apos;s Dairy Twist', '', '', 42.479825, -82.958237, 0, ''];</v>
+        <v>y[31] = [1, 'KC&amp;apos;s Dairy Twist', '', '', 42.479825, -82.958237, 0, 'Ice Cream, Family friendly'];</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H33" s="4">
         <v>0</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[32] = [1, 'Marz Bar', '', '', 42.479803, -82.964470, 0, ''];</v>
+        <v>y[32] = [1, 'Marz Bar', '', '', 42.479803, -82.964470, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B34" s="4">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="H34" s="4">
         <v>0</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[33] = [1, 'Legend&amp;apos;s Coney Express', '', '', 42.465404, -82.937518, 0, ''];</v>
+        <v>y[33] = [1, 'Legend&amp;apos;s Coney Express', '', '', 42.465404, -82.937518, 0, 'American, Sandwiches'];</v>
       </c>
       <c r="B35" s="4">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="H35" s="4">
         <v>0</v>
       </c>
       <c r="K35" s="4">
         <v>1</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2007,13 +2109,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="H36" s="4">
         <v>0</v>
@@ -2025,49 +2127,55 @@
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[35] = [1, 'McGee&amp;apos;s Lounge', '', '', 42.459181, -82.961050, 0, ''];</v>
+        <v>y[35] = [1, 'McGee&amp;apos;s Lounge', '', '', 42.459181, -82.961050, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="H37" s="4">
         <v>0</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[36] = [1, 'O&amp;apos;Hara&amp;apos;s Irish Pub', '', '', 42.479876, -82.956645, 0, ''];</v>
+        <v>y[36] = [1, 'O&amp;apos;Hara&amp;apos;s Irish Pub', '', '', 42.479876, -82.956645, 0, 'American, Sandwiches, Alcohol'];</v>
       </c>
       <c r="B38" s="4">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="H38" s="4">
         <v>0</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[37] = [1, 'Panda', '', '', , , 0, ''];</v>
+        <v>y[37] = [1, 'Panda', '', '', , , 0, 'Chinese'];</v>
       </c>
       <c r="B39" s="4">
         <v>1</v>
@@ -2078,6 +2186,9 @@
       <c r="H39" s="4">
         <v>0</v>
       </c>
+      <c r="L39" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="str">
@@ -2091,10 +2202,10 @@
         <v>27</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H40" s="4">
         <v>0</v>
@@ -2106,7 +2217,7 @@
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[39] = [1, 'Plaza Mexico', '', '', 42.465058, -82.931126, 0, ''];</v>
+        <v>y[39] = [1, 'Plaza Mexico', '', '', 42.465058, -82.931126, 0, 'Mexican'];</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
@@ -2115,40 +2226,46 @@
         <v>28</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H41" s="4">
         <v>0</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[40] = [1, 'Popeye&amp;apos;s', '', '', 42.465148, -82.928295, 0, ''];</v>
+        <v>y[40] = [1, 'Popeye&amp;apos;s', '', '', 42.465148, -82.928295, 0, 'American'];</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H42" s="4">
         <v>0</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[41] = [1, 'Scoreboard Sports Bar &amp; Grill', '', '', 42.480226, -82.955936, 0, ''];</v>
+        <v>y[41] = [1, 'Scoreboard Sports Bar &amp; Grill', '', '', 42.480226, -82.955936, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
@@ -2157,19 +2274,22 @@
         <v>29</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H43" s="4">
         <v>0</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[42] = [1, 'Shawarma Express', '', '', 42.479489, -82.948824, 0, ''];</v>
+        <v>y[42] = [1, 'Shawarma Express', '', '', 42.479489, -82.948824, 0, 'Mediterranean'];</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
@@ -2178,19 +2298,22 @@
         <v>30</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H44" s="4">
         <v>0</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[43] = [1, 'Shish Kabob', '', '', 42.460782, -82.960984, 0, ''];</v>
+        <v>y[43] = [1, 'Shish Kabob', '', '', 42.460782, -82.960984, 0, 'Mediterranean'];</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
@@ -2199,40 +2322,46 @@
         <v>31</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H45" s="4">
         <v>0</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[44] = [1, 'Snooker&amp;apos;s Pool &amp; Pub', '', '', 42.459500, -82.932982, 0, ''];</v>
+        <v>y[44] = [1, 'Snooker&amp;apos;s Pool &amp; Pub', '', '', 42.459500, -82.932982, 0, 'Bar, Alcohol, American'];</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H46" s="4">
         <v>0</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[45] = [1, 'Subway', '', '', 42.465146, -82.929948, 0, ''];</v>
+        <v>y[45] = [1, 'Subway', '', '', 42.465146, -82.929948, 0, 'Sandwiches'];</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
@@ -2241,19 +2370,22 @@
         <v>32</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H47" s="4">
         <v>0</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[46] = [1, 'Subway', '', '', 42.463094, -82.960277, 0, ''];</v>
+        <v>y[46] = [1, 'Subway', '', '', 42.463094, -82.960277, 0, 'Sandwiches'];</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -2262,19 +2394,22 @@
         <v>32</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H48" s="4">
         <v>0</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[47] = [1, 'Taco Bell', '', '', 42.465354, -82.938304, 0, ''];</v>
+        <v>y[47] = [1, 'Taco Bell', '', '', 42.465354, -82.938304, 0, 'Mexican'];</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
@@ -2283,19 +2418,22 @@
         <v>33</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H49" s="4">
         <v>0</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[48] = [1, 'Wah Hong Chop Suey', '', '', 42.450736, -82.942593, 0, ''];</v>
+        <v>y[48] = [1, 'Wah Hong Chop Suey', '', '', 42.450736, -82.942593, 0, 'Chinese'];</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -2304,40 +2442,46 @@
         <v>34</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H50" s="4">
         <v>0</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[49] = [1, 'Wendy&amp;apos;s', '', '', 42.465537, -82.934832, 0, ''];</v>
+        <v>y[49] = [1, 'Wendy&amp;apos;s', '', '', 42.465537, -82.934832, 0, 'American, Sandwiches'];</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H51" s="4">
         <v>0</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[50] = [1, 'Western', '', '', 42.456441, -82.963968, 0, ''];</v>
+        <v>y[50] = [1, 'Western', '', '', 42.456441, -82.963968, 0, 'American'];</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
@@ -2346,19 +2490,22 @@
         <v>35</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H52" s="4">
         <v>0</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[51] = [1, 'White Castle', '', '', 42.450380, -82.968444, 0, ''];</v>
+        <v>y[51] = [1, 'White Castle', '', '', 42.450380, -82.968444, 0, 'American'];</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
@@ -2367,19 +2514,22 @@
         <v>36</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H53" s="4">
         <v>0</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[52] = [1, 'Milestone Grill', '', '', 42.465453, -82.937006, 0, 'Pizza'];</v>
+        <v>y[52] = [1, 'Milestone Grill', '', '', 42.465453, -82.937006, 0, 'Pizza, Bar, Alcohol, Mediterranean'];</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -2388,16 +2538,16 @@
         <v>47</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H54" s="4">
         <v>0</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>7</v>
+        <v>243</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -2409,7 +2559,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H55" s="4">
         <v>0</v>
@@ -2418,7 +2568,7 @@
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[54] = [1, 'Wing Stop', '', '', 42.463214, -82.960226, 0, ''];</v>
+        <v>y[54] = [1, 'Wing Stop', '', '', 42.463214, -82.960226, 0, 'American'];</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
@@ -2427,76 +2577,88 @@
         <v>48</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H56" s="4">
         <v>0</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[55] = [1, 'Granma&amp;apos;s House of Pancakes', '', '', 42.465341, -82.943988, 0, ''];</v>
+        <v>y[55] = [1, 'Granma&amp;apos;s House of Pancakes', '', '', 42.465341, -82.943988, 0, 'American, Breakfast'];</v>
       </c>
       <c r="B57" s="4">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H57" s="4">
         <v>0</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[56] = [1, 'Josephine&amp;apos;s Soul Food', '', '', 42.464982, -82.935152, 0, ''];</v>
+        <v>y[56] = [1, 'Josephine&amp;apos;s Soul Food', '', '', 42.464982, -82.935152, 0, 'BBQ'];</v>
       </c>
       <c r="B58" s="4">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H58" s="4">
         <v>0</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[57] = [1, 'Sullivan&amp;apos;s', '', '', 42.465000, -82.932341, 0, ''];</v>
+        <v>y[57] = [1, 'Sullivan&amp;apos;s', '', '', 42.465000, -82.932341, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B59" s="4">
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H59" s="4">
         <v>0</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -2511,10 +2673,10 @@
         <v>49</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H60" s="4">
         <v>0</v>
@@ -2550,10 +2712,10 @@
         <v>51</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H62" s="4">
         <v>0</v>
@@ -2565,43 +2727,49 @@
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[61] = [1, 'East Detroit Bakery', '', '', 42.464771, -82.941100, 0, ''];</v>
+        <v>y[61] = [1, 'East Detroit Bakery', '', '', 42.464771, -82.941100, 0, 'Bakery'];</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L63" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[62] = [1, 'Cup Cakes &amp; Ice Cream Kids', '', '', 42.464743, -82.940718, 0, ''];</v>
+        <v>y[62] = [1, 'Cup Cakes &amp; Ice Cream Kids', '', '', 42.464743, -82.940718, 0, 'Bakery'];</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -2610,19 +2778,19 @@
         <v>y[63] = [1, 'Taormina&amp;apos;s Pizza &amp; Ice Cream', '', '', 42.472294, -82.967218, 0, 'Pizza'];</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>7</v>
@@ -2630,7 +2798,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Changed Marz Bar to Last Call Bar and Josephine Soul Food to 10x Better Soul Food. Delete any duplicates.
</commit_message>
<xml_diff>
--- a/EATSpointe.xlsx
+++ b/EATSpointe.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="244">
   <si>
     <t>Restaurant</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Family friendly</t>
   </si>
   <si>
-    <t>Diner</t>
-  </si>
-  <si>
     <t>Sandwiches</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>Bakery</t>
   </si>
   <si>
-    <t>Marz Bar</t>
-  </si>
-  <si>
     <t>Cup Cakes &amp; Ice Cream Kids</t>
   </si>
   <si>
@@ -272,9 +266,6 @@
     <t>Sullivan&amp;apos;s</t>
   </si>
   <si>
-    <t>Josephine&amp;apos;s Soul Food</t>
-  </si>
-  <si>
     <t>Granma&amp;apos;s House of Pancakes</t>
   </si>
   <si>
@@ -762,6 +753,9 @@
   </si>
   <si>
     <t>Diner, American, Coffee, Breakfast</t>
+  </si>
+  <si>
+    <t>Last Call Bar</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1134,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>16</v>
@@ -1155,10 +1149,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
@@ -1191,13 +1185,13 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
@@ -1212,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>38</v>
@@ -1220,32 +1214,32 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
-        <f t="shared" ref="A3:A65" si="0">CONCATENATE("y[",ROW()-2,"] = [",B3,", '",C3,"', '",D3,"', '",E3,"', ",F3,", ",G3,", ",H3,", '",L3,"'];")</f>
+        <f t="shared" ref="A3:A64" si="0">CONCATENATE("y[",ROW()-2,"] = [",B3,", '",C3,"', '",D3,"', '",E3,"', ",F3,", ",G3,", ",H3,", '",L3,"'];")</f>
         <v>y[1] = [1, 'Villa Restaurant &amp; Pizzeria', '', '21311 Gratiot Avenue', 42.454643, -82.965264, 1, 'Italian, Pizza, Alcohol, Family friendly'];</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H3" s="4">
         <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1257,22 +1251,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>40</v>
@@ -1290,19 +1284,19 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H5" s="4">
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>8</v>
@@ -1317,25 +1311,25 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1347,16 +1341,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H7" s="4">
         <v>1</v>
@@ -1377,16 +1371,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H8" s="4">
         <v>1</v>
@@ -1395,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>7</v>
@@ -1413,22 +1407,22 @@
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H9" s="4">
         <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1440,16 +1434,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
@@ -1467,16 +1461,16 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H11" s="4">
         <v>1</v>
@@ -1506,7 +1500,7 @@
         <v>7</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1521,19 +1515,19 @@
         <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H13" s="4">
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>46</v>
@@ -1551,22 +1545,22 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H14" s="4">
         <v>1</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1578,16 +1572,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H15" s="4">
         <v>1</v>
@@ -1602,397 +1596,394 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[14] = [1, '10x Better Soul Food', '', '', , , 0, 'BBQ'];</v>
+        <v>y[14] = [1, 'Adriana&amp;apos;s Kitchen', '', '', 42.465112, -82.948927, 0, 'American'];</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>95</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="H16" s="4">
         <v>0</v>
       </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>1</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>57</v>
+      <c r="L16" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[15] = [1, 'Adriana&amp;apos;s Kitchen', '', '', 42.465112, -82.948927, 0, 'American'];</v>
+        <v>y[15] = [1, 'Andary&amp;apos;s Grill &amp; Deli', '', '', 42.470411, -82.954819, 0, 'American, Coffee, Family friendly'];</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H17" s="4">
         <v>0</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>38</v>
+        <v>230</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>54</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[16] = [1, 'Andary&amp;apos;s Grill &amp; Deli', '', '', 42.470411, -82.954819, 0, 'American, Coffee, Family friendly'];</v>
+        <v>y[16] = [1, 'Big Boy', '', '', 42.465559, -82.958383, 0, 'American, Sandwiches, Coffee'];</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H18" s="4">
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[17] = [1, 'Big Boy', '', '', 42.465559, -82.958383, 0, 'American, Sandwiches, Coffee'];</v>
+        <v>y[17] = [1, 'Boney Moroney Bar', '', '', 42.456316, -82.962807, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H19" s="4">
         <v>0</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[18] = [1, 'Boney Moroney Bar', '', '', 42.456316, -82.962807, 0, 'Bar, Alcohol'];</v>
+        <v>y[18] = [1, 'Bread Basket Deli', '', '', 42.450935, -82.940886, 0, 'Sandwiches'];</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H20" s="4">
         <v>0</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>229</v>
+        <v>55</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[19] = [1, 'Bread Basket Deli', '', '', 42.450935, -82.940886, 0, 'Sandwiches'];</v>
+        <v>y[19] = [1, 'Burger King', '', '', 42.450942, -82.966426, 0, 'Sandwiches'];</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H21" s="4">
         <v>0</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[20] = [1, 'Burger King', '', '', 42.450942, -82.966426, 0, 'Sandwiches'];</v>
+        <v>y[20] = [1, 'China Wok', '', '', 42.462667, -82.929915, 0, 'Chinese'];</v>
       </c>
       <c r="B22" s="4">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H22" s="4">
         <v>0</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[21] = [1, 'China Wok', '', '', 42.462667, -82.929915, 0, 'Chinese'];</v>
+        <v>y[21] = [1, 'Coffee Break Café', '', '', 42.479804, -82.920525, 0, 'Coffee'];</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H23" s="4">
         <v>0</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[22] = [1, 'Coffee Break Café', '', '', 42.479804, -82.920525, 0, 'Coffee'];</v>
+        <v>y[22] = [1, 'Dairy Queen Brazier', '', '', 42.465111, -82.944537, 0, 'American, Sandwiches, Family friendly, Ice Cream'];</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H24" s="4">
         <v>0</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>39</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[23] = [1, 'Dairy Queen Brazier', '', '', 42.465111, -82.944537, 0, 'American, Sandwiches, Family friendly, Ice Cream'];</v>
+        <v>y[23] = [1, 'Domino&amp;apos;s Pizza', '', '', 42.479924, -82.964993, 0, 'Pizza'];</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H25" s="4">
         <v>0</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>236</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[24] = [1, 'Domino&amp;apos;s Pizza', '', '', 42.479924, -82.964993, 0, 'Pizza'];</v>
+        <v>y[24] = [1, 'Eastpointe Pub', '', '', 42.465298, -82.924711, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H26" s="4">
         <v>0</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>7</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[25] = [1, 'Eastpointe Pub', '', '', 42.465298, -82.924711, 0, 'Bar, Alcohol'];</v>
+        <v>y[25] = [1, 'Five Guys &amp; Fries', '', '', 42.464157, -82.959707, 0, 'Sandwiches'];</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="H27" s="4">
         <v>0</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>229</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[26] = [1, 'Five Guys &amp; Fries', '', '', 42.464157, -82.959707, 0, 'Sandwiches'];</v>
+        <v>y[26] = [1, 'Guiseppe&amp;apos;s Bakery', '', '', 42.458315, -82.934028, 0, 'Bakery'];</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="H28" s="4">
         <v>0</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[27] = [1, 'Guiseppe&amp;apos;s Bakery', '', '', 42.458315, -82.934028, 0, 'Bakery'];</v>
+        <v>y[27] = [1, 'Happy Garden', '', '', 42.462424, -82.958903, 0, 'Chinese'];</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H29" s="4">
         <v>0</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[28] = [1, 'Happy Garden', '', '', 42.462424, -82.958903, 0, 'Chinese'];</v>
+        <v>y[28] = [1, 'Happy&amp;apos;s Pizza', '', '', 42.471669, -82.952741, 0, 'Pizza'];</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H30" s="4">
         <v>0</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[29] = [1, 'Happy&amp;apos;s Pizza', '', '', 42.471669, -82.952741, 0, 'Pizza'];</v>
+        <v>y[29] = [1, 'Jet&amp;apos;s Pizza', '', '', 42.479976, -82.918491, 0, 'Pizza'];</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H31" s="4">
         <v>0</v>
@@ -2004,364 +1995,364 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[30] = [1, 'Jet&amp;apos;s Pizza', '', '', 42.479976, -82.918491, 0, 'Pizza'];</v>
+        <v>y[30] = [1, 'KC&amp;apos;s Dairy Twist', '', '', 42.479825, -82.958237, 0, 'Ice Cream, Family friendly'];</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H32" s="4">
         <v>0</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>7</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[31] = [1, 'KC&amp;apos;s Dairy Twist', '', '', 42.479825, -82.958237, 0, 'Ice Cream, Family friendly'];</v>
+        <v>y[31] = [1, 'Last Call Bar', '', '', 42.479803, -82.964470, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>92</v>
+        <v>243</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="H33" s="4">
         <v>0</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[32] = [1, 'Marz Bar', '', '', 42.479803, -82.964470, 0, 'Bar, Alcohol'];</v>
+        <v>y[32] = [1, 'Legend&amp;apos;s Coney Express', '', '', 42.465404, -82.937518, 0, 'American, Sandwiches'];</v>
       </c>
       <c r="B34" s="4">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H34" s="4">
         <v>0</v>
       </c>
+      <c r="K34" s="4">
+        <v>1</v>
+      </c>
       <c r="L34" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[33] = [1, 'Legend&amp;apos;s Coney Express', '', '', 42.465404, -82.937518, 0, 'American, Sandwiches'];</v>
+        <v>y[33] = [1, 'Little Caesar&amp;apos;s', '', '', 42.479923, -82.955558, 0, 'Pizza'];</v>
       </c>
       <c r="B35" s="4">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H35" s="4">
         <v>0</v>
       </c>
-      <c r="K35" s="4">
-        <v>1</v>
-      </c>
       <c r="L35" s="1" t="s">
-        <v>238</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[34] = [1, 'Little Caesar&amp;apos;s', '', '', 42.479923, -82.955558, 0, 'Pizza'];</v>
+        <v>y[34] = [1, 'McGee&amp;apos;s Lounge', '', '', 42.459181, -82.961050, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H36" s="4">
         <v>0</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>7</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[35] = [1, 'McGee&amp;apos;s Lounge', '', '', 42.459181, -82.961050, 0, 'Bar, Alcohol'];</v>
+        <v>y[35] = [1, 'O&amp;apos;Hara&amp;apos;s Irish Pub', '', '', 42.479876, -82.956645, 0, 'American, Sandwiches, Alcohol'];</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H37" s="4">
         <v>0</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[36] = [1, 'O&amp;apos;Hara&amp;apos;s Irish Pub', '', '', 42.479876, -82.956645, 0, 'American, Sandwiches, Alcohol'];</v>
+        <v>y[36] = [1, 'Panda', '', '', , , 0, 'Chinese'];</v>
       </c>
       <c r="B38" s="4">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>177</v>
+        <v>26</v>
       </c>
       <c r="H38" s="4">
         <v>0</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>239</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[37] = [1, 'Panda', '', '', , , 0, 'Chinese'];</v>
+        <v>y[37] = [1, 'Pizza Square', '', '', 42.453855, -82.938276, 0, 'Pizza'];</v>
       </c>
       <c r="B39" s="4">
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="H39" s="4">
         <v>0</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[38] = [1, 'Pizza Square', '', '', 42.453855, -82.938276, 0, 'Pizza'];</v>
+        <v>y[38] = [1, 'Plaza Mexico', '', '', 42.465058, -82.931126, 0, 'Mexican'];</v>
       </c>
       <c r="B40" s="4">
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H40" s="4">
         <v>0</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[39] = [1, 'Plaza Mexico', '', '', 42.465058, -82.931126, 0, 'Mexican'];</v>
+        <v>y[39] = [1, 'Popeye&amp;apos;s', '', '', 42.465148, -82.928295, 0, 'American'];</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H41" s="4">
         <v>0</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[40] = [1, 'Popeye&amp;apos;s', '', '', 42.465148, -82.928295, 0, 'American'];</v>
+        <v>y[40] = [1, 'Scoreboard Sports Bar &amp; Grill', '', '', 42.480226, -82.955936, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H42" s="4">
         <v>0</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>38</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[41] = [1, 'Scoreboard Sports Bar &amp; Grill', '', '', 42.480226, -82.955936, 0, 'Bar, Alcohol'];</v>
+        <v>y[41] = [1, 'Shawarma Express', '', '', 42.479489, -82.948824, 0, 'Mediterranean'];</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H43" s="4">
         <v>0</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[42] = [1, 'Shawarma Express', '', '', 42.479489, -82.948824, 0, 'Mediterranean'];</v>
+        <v>y[42] = [1, 'Shish Kabob', '', '', 42.460782, -82.960984, 0, 'Mediterranean'];</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H44" s="4">
         <v>0</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[43] = [1, 'Shish Kabob', '', '', 42.460782, -82.960984, 0, 'Mediterranean'];</v>
+        <v>y[43] = [1, 'Snooker&amp;apos;s Pool &amp; Pub', '', '', 42.459500, -82.932982, 0, 'Bar, Alcohol, American'];</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H45" s="4">
         <v>0</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[44] = [1, 'Snooker&amp;apos;s Pool &amp; Pub', '', '', 42.459500, -82.932982, 0, 'Bar, Alcohol, American'];</v>
+        <v>y[44] = [1, 'Subway', '', '', 42.465146, -82.929948, 0, 'Sandwiches'];</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H46" s="4">
         <v>0</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>241</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[45] = [1, 'Subway', '', '', 42.465146, -82.929948, 0, 'Sandwiches'];</v>
+        <v>y[45] = [1, 'Subway', '', '', 42.463094, -82.960277, 0, 'Sandwiches'];</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
@@ -2370,130 +2361,130 @@
         <v>32</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H47" s="4">
         <v>0</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[46] = [1, 'Subway', '', '', 42.463094, -82.960277, 0, 'Sandwiches'];</v>
+        <v>y[46] = [1, 'Taco Bell', '', '', 42.465354, -82.938304, 0, 'Mexican'];</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H48" s="4">
         <v>0</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[47] = [1, 'Taco Bell', '', '', 42.465354, -82.938304, 0, 'Mexican'];</v>
+        <v>y[47] = [1, 'Wah Hong Chop Suey', '', '', 42.450736, -82.942593, 0, 'Chinese'];</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H49" s="4">
         <v>0</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[48] = [1, 'Wah Hong Chop Suey', '', '', 42.450736, -82.942593, 0, 'Chinese'];</v>
+        <v>y[48] = [1, 'Wendy&amp;apos;s', '', '', 42.465537, -82.934832, 0, 'American, Sandwiches'];</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H50" s="4">
         <v>0</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>40</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[49] = [1, 'Wendy&amp;apos;s', '', '', 42.465537, -82.934832, 0, 'American, Sandwiches'];</v>
+        <v>y[49] = [1, 'Western', '', '', 42.456441, -82.963968, 0, 'American'];</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H51" s="4">
         <v>0</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>238</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[50] = [1, 'Western', '', '', 42.456441, -82.963968, 0, 'American'];</v>
+        <v>y[50] = [1, 'White Castle', '', '', 42.450380, -82.968444, 0, 'American'];</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H52" s="4">
         <v>0</v>
@@ -2505,315 +2496,291 @@
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[51] = [1, 'White Castle', '', '', 42.450380, -82.968444, 0, 'American'];</v>
+        <v>y[51] = [1, 'Milestone Grill', '', '', 42.465453, -82.937006, 0, 'Pizza, Bar, Alcohol, Mediterranean'];</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H53" s="4">
         <v>0</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>38</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[52] = [1, 'Milestone Grill', '', '', 42.465453, -82.937006, 0, 'Pizza, Bar, Alcohol, Mediterranean'];</v>
+        <v>y[52] = [1, 'Ashby&amp;apos;s', '', '', , , 0, ''];</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>192</v>
+        <v>81</v>
       </c>
       <c r="H54" s="4">
         <v>0</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[53] = [1, 'Ashby&amp;apos;s', '', '', , , 0, ''];</v>
+        <v>y[53] = [1, 'Wing Stop', '', '', 42.463214, -82.960226, 0, 'American'];</v>
       </c>
       <c r="B55" s="4">
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>84</v>
+        <v>48</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="H55" s="4">
         <v>0</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[54] = [1, 'Wing Stop', '', '', 42.463214, -82.960226, 0, 'American'];</v>
+        <v>y[54] = [1, 'Granma&amp;apos;s House of Pancakes', '', '', 42.465341, -82.943988, 0, 'American, Breakfast'];</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H56" s="4">
         <v>0</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>38</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[55] = [1, 'Granma&amp;apos;s House of Pancakes', '', '', 42.465341, -82.943988, 0, 'American, Breakfast'];</v>
+        <v>y[55] = [1, '10x Better Soul Food', '', '', 42.464982, -82.935152, 0, 'BBQ'];</v>
       </c>
       <c r="B57" s="4">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H57" s="4">
         <v>0</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>244</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[56] = [1, 'Josephine&amp;apos;s Soul Food', '', '', 42.464982, -82.935152, 0, 'BBQ'];</v>
+        <v>y[56] = [1, 'Sullivan&amp;apos;s', '', '', 42.465000, -82.932341, 0, 'Bar, Alcohol'];</v>
       </c>
       <c r="B58" s="4">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H58" s="4">
         <v>0</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>57</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[57] = [1, 'Sullivan&amp;apos;s', '', '', 42.465000, -82.932341, 0, 'Bar, Alcohol'];</v>
+        <v>y[57] = [1, 'Di Frattelli Pizza', '', '', 42.465315, -82.924976, 0, 'Pizza'];</v>
       </c>
       <c r="B59" s="4">
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H59" s="4">
         <v>0</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>229</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[58] = [1, 'Di Frattelli Pizza', '', '', 42.465315, -82.924976, 0, 'Pizza'];</v>
+        <v>y[58] = [1, 'Gratiot Avenue Memory Lane Café', '', '', , , 0, ''];</v>
       </c>
       <c r="B60" s="4">
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>212</v>
+        <v>50</v>
       </c>
       <c r="H60" s="4">
         <v>0</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[59] = [1, 'Gratiot Avenue Memory Lane Café', '', '', , , 0, ''];</v>
+        <v>y[59] = [1, 'Passport Pizza', '', '', 42.480257, -82.949271, 0, 'Pizza'];</v>
       </c>
       <c r="B61" s="4">
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="H61" s="4">
         <v>0</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[60] = [1, 'Passport Pizza', '', '', 42.480257, -82.949271, 0, 'Pizza'];</v>
-      </c>
-      <c r="B62" s="4">
-        <v>1</v>
+        <v>y[60] = [1, 'East Detroit Bakery', '', '', 42.464771, -82.941100, 0, 'Bakery'];</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H62" s="4">
-        <v>0</v>
+        <v>216</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[61] = [1, 'East Detroit Bakery', '', '', 42.464771, -82.941100, 0, 'Bakery'];</v>
+        <v>y[61] = [1, 'Cup Cakes &amp; Ice Cream Kids', '', '', 42.464743, -82.940718, 0, 'Bakery'];</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H63" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H63" s="4" t="s">
+      <c r="L63" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>y[62] = [1, 'Cup Cakes &amp; Ice Cream Kids', '', '', 42.464743, -82.940718, 0, 'Bakery'];</v>
+        <v>y[62] = [1, 'Taormina&amp;apos;s Pizza &amp; Ice Cream', '', '', 42.472294, -82.967218, 0, 'Pizza'];</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>y[63] = [1, 'Taormina&amp;apos;s Pizza &amp; Ice Cream', '', '', 42.472294, -82.967218, 0, 'Pizza'];</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H65" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="L65" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="9" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
     </row>
   </sheetData>
   <sortState ref="M2:M12">
     <sortCondition ref="M2"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C66:E66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added 6 new locations
</commit_message>
<xml_diff>
--- a/EATSpointe.xlsx
+++ b/EATSpointe.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="282">
   <si>
     <t>Restaurant</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Plaza Mexico</t>
   </si>
   <si>
-    <t>Scoreboard Sports Bar &amp; Grill</t>
-  </si>
-  <si>
     <t>Shawarma Express</t>
   </si>
   <si>
@@ -817,6 +814,63 @@
   </si>
   <si>
     <t>Elena&amp;apos;s Pizza</t>
+  </si>
+  <si>
+    <t>Little Italy Pizza</t>
+  </si>
+  <si>
+    <t>East Wind Chinese Food</t>
+  </si>
+  <si>
+    <t>Friendly Family Restaurant</t>
+  </si>
+  <si>
+    <t>Boston Z</t>
+  </si>
+  <si>
+    <t>Fairway Bar and Grill</t>
+  </si>
+  <si>
+    <t>Homestead Bakery and Deli</t>
+  </si>
+  <si>
+    <t>Detroit Wing Company</t>
+  </si>
+  <si>
+    <t>-82.920517</t>
+  </si>
+  <si>
+    <t>42.479858</t>
+  </si>
+  <si>
+    <t>42.479882</t>
+  </si>
+  <si>
+    <t>-82.918019</t>
+  </si>
+  <si>
+    <t>42.479790</t>
+  </si>
+  <si>
+    <t>-82.921024</t>
+  </si>
+  <si>
+    <t>-82.920172</t>
+  </si>
+  <si>
+    <t>42.479802</t>
+  </si>
+  <si>
+    <t>-82.918303</t>
+  </si>
+  <si>
+    <t>42.479944</t>
+  </si>
+  <si>
+    <t>42.465293</t>
+  </si>
+  <si>
+    <t>-82.940838</t>
   </si>
 </sst>
 </file>
@@ -886,7 +940,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1169,11 +1223,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C70" sqref="C70"/>
+      <selection pane="topRight" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1196,7 +1250,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>16</v>
@@ -1211,10 +1265,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
@@ -1226,13 +1280,13 @@
         <v>4</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1247,13 +1301,13 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
@@ -1268,10 +1322,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1283,25 +1337,25 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H3" s="4">
         <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1313,22 +1367,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>8</v>
@@ -1346,22 +1400,22 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H5" s="4">
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1373,25 +1427,25 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1403,22 +1457,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H7" s="4">
         <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>7</v>
@@ -1433,16 +1487,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H8" s="4">
         <v>1</v>
@@ -1451,10 +1505,10 @@
         <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1469,19 +1523,19 @@
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H9" s="4">
         <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1493,25 +1547,25 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1523,25 +1577,25 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H11" s="4">
         <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1556,19 +1610,19 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="H12" s="4">
         <v>1</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1583,22 +1637,22 @@
         <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H13" s="4">
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1613,22 +1667,22 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H14" s="4">
         <v>1</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1640,25 +1694,25 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H15" s="4">
         <v>1</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1670,19 +1724,19 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H16" s="4">
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1697,19 +1751,19 @@
         <v>17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H17" s="4">
         <v>0</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1724,19 +1778,19 @@
         <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H18" s="4">
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1751,19 +1805,19 @@
         <v>19</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H19" s="4">
         <v>0</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1778,16 +1832,16 @@
         <v>20</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H20" s="4">
         <v>0</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1802,16 +1856,16 @@
         <v>21</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H21" s="4">
         <v>0</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1826,16 +1880,16 @@
         <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H22" s="4">
         <v>0</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -1847,19 +1901,19 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H23" s="4">
         <v>0</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1871,19 +1925,19 @@
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H24" s="4">
         <v>0</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1898,16 +1952,16 @@
         <v>23</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H25" s="4">
         <v>0</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1922,16 +1976,16 @@
         <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H26" s="4">
         <v>0</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -1943,19 +1997,19 @@
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H27" s="4">
         <v>0</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -1970,16 +2024,16 @@
         <v>25</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H28" s="4">
         <v>0</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -1991,19 +2045,19 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H29" s="4">
         <v>0</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -2015,19 +2069,19 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H30" s="4">
         <v>0</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -2039,19 +2093,19 @@
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H31" s="4">
         <v>0</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -2063,19 +2117,19 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H32" s="4">
         <v>0</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -2087,13 +2141,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H33" s="4">
         <v>0</v>
@@ -2102,31 +2156,31 @@
         <v>1</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="str">
-        <f t="shared" ref="A34:A66" si="1">CONCATENATE("y[",ROW()-2,"] = [",B34,", '",C34,"', '",D34,"', '",E34,"', ",F34,", ",G34,", ",H34,", '",L34,"'];")</f>
+        <f t="shared" ref="A34:A68" si="1">CONCATENATE("y[",ROW()-2,"] = [",B34,", '",C34,"', '",D34,"', '",E34,"', ",F34,", ",G34,", ",H34,", '",L34,"'];")</f>
         <v>y[32] = [1, 'Little Caesar&amp;apos;s', '', '', 42.479923, -82.955558, 0, 'Take-Out, Pizza'];</v>
       </c>
       <c r="B34" s="4">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H34" s="4">
         <v>0</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2138,19 +2192,19 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H35" s="4">
         <v>0</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2162,19 +2216,19 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H36" s="4">
         <v>0</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -2189,16 +2243,16 @@
         <v>26</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="H37" s="4">
         <v>0</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2213,16 +2267,16 @@
         <v>27</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H38" s="4">
         <v>0</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2237,16 +2291,16 @@
         <v>28</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H39" s="4">
         <v>0</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -2258,43 +2312,43 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H40" s="4">
         <v>0</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>y[39] = [1, 'Scoreboard Sports Bar &amp; Grill', '', '', 42.480226, -82.955936, 0, 'Dine-In, Alcohol, Bar'];</v>
+        <v>y[39] = [1, 'Boston Z', '', '', 42.480226, -82.955936, 0, 'Dine-In, Alcohol, Bar'];</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>29</v>
+        <v>266</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H41" s="4">
         <v>0</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -2306,19 +2360,19 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H42" s="4">
         <v>0</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
@@ -2330,19 +2384,19 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H43" s="4">
         <v>0</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -2354,19 +2408,19 @@
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H44" s="4">
         <v>0</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2378,19 +2432,19 @@
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H45" s="4">
         <v>0</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2402,19 +2456,19 @@
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H46" s="4">
         <v>0</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -2426,19 +2480,19 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H47" s="4">
         <v>0</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -2450,19 +2504,19 @@
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H48" s="4">
         <v>0</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -2474,19 +2528,19 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H49" s="4">
         <v>0</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -2498,19 +2552,19 @@
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H50" s="4">
         <v>0</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -2522,19 +2576,19 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H51" s="4">
         <v>0</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -2546,19 +2600,19 @@
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H52" s="4">
         <v>0</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -2570,19 +2624,19 @@
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="H53" s="4">
         <v>0</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -2594,19 +2648,19 @@
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H54" s="4">
         <v>0</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -2618,19 +2672,19 @@
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H55" s="4">
         <v>0</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -2645,16 +2699,16 @@
         <v>15</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H56" s="4">
         <v>0</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -2666,19 +2720,19 @@
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H57" s="4">
         <v>0</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -2690,19 +2744,19 @@
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H58" s="4">
         <v>0</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -2714,19 +2768,19 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H59" s="4">
         <v>0</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -2735,22 +2789,22 @@
         <v>y[58] = [1, 'East Detroit Bakery', '', '', 42.464771, -82.941100, 0, 'Take-Out, Bakery, Coffee'];</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H60" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="L60" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -2759,22 +2813,22 @@
         <v>y[59] = [1, 'Taormina&amp;apos;s Pizza &amp; Ice Cream', '', '', 42.472294, -82.967218, 0, 'Dine-In, Take-Out, Pizza'];</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H61" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="L61" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -2783,45 +2837,189 @@
         <v>y[60] = [1, 'Elena&amp;apos;s Pizza', '', '18830 E. 9 Mile Road', 42.465309, -82.924987, 0, 'Take-Out, Pizza'];</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H62" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="L62" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>y[61] = [1, 'Little Italy Pizza', '', '', 42.479858, -82.920517, 0, 'Take-Out, Pizza'];</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>223</v>
+      <c r="F63" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
+      <c r="A64" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>y[62] = [1, 'East Wind Chinese Food', '', '', 42.479802, -82.920172, 0, 'Dine-In, Take-Out, Chinese'];</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>y[63] = [1, 'Friendly Family Restaurant', '', '', 42.479790, -82.921024, 0, 'Dine-In, Take-Out, American, Kids Menu'];</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>y[64] = [1, 'Homestead Bakery and Deli', '', '', 42.479944, -82.918303, 0, 'Take-Out, Bakery'];</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>y[65] = [1, 'Fairway Bar and Grill', '', '', 42.479882, -82.918019, 0, 'Dine-In, Alcohol, Bar'];</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>y[66] = [1, 'Detroit Wing Company', '', '', 42.465293, -82.940838, 0, 'Dine-In, Take-Out, American'];</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="M2:M12">
     <sortCondition ref="M2"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="A70:C70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2840,7 +3038,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>16</v>
@@ -2855,10 +3053,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
@@ -2870,13 +3068,13 @@
         <v>4</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2888,13 +3086,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H2" s="4">
         <v>0</v>
@@ -2903,10 +3101,10 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>